<commit_message>
define separate parameter for path to firmware
</commit_message>
<xml_diff>
--- a/domains.xlsx
+++ b/domains.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27322"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27729"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28680" windowHeight="17500" tabRatio="500"/>
+    <workbookView xWindow="480" yWindow="480" windowWidth="25120" windowHeight="15040" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="site.conf" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <connection id="1" name="profile.csv" type="6" refreshedVersion="0" background="1" saveData="1">
-    <textPr fileType="mac" codePage="10000" sourceFile="Macintosh HD:Users:klausjerwan:Documents:Freie Infrastruktur:Freifunk:dev:profile.csv" decimal="," thousands="." tab="0" space="1" consecutive="1">
+    <textPr fileType="mac" sourceFile="Macintosh HD:Users:klausjerwan:Documents:Freie Infrastruktur:Freifunk:dev:profile.csv" decimal="," thousands="." tab="0" space="1" consecutive="1">
       <textFields count="7">
         <textField/>
         <textField/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="157">
   <si>
     <t>ffhpd01</t>
   </si>
@@ -434,6 +434,81 @@
   </si>
   <si>
     <t>ABT-</t>
+  </si>
+  <si>
+    <t>BSSID</t>
+  </si>
+  <si>
+    <t>02:d1:11:37:fc:39</t>
+  </si>
+  <si>
+    <t>02:d1:11:37:fc:40</t>
+  </si>
+  <si>
+    <t>02:d1:11:37:fc:41</t>
+  </si>
+  <si>
+    <t>02:d1:11:37:fc:42</t>
+  </si>
+  <si>
+    <t>02:d1:11:37:fc:43</t>
+  </si>
+  <si>
+    <t>02:d1:11:37:fc:44</t>
+  </si>
+  <si>
+    <t>02:d1:11:37:fc:45</t>
+  </si>
+  <si>
+    <t>02:d1:11:37:fc:46</t>
+  </si>
+  <si>
+    <t>02:d1:11:37:fc:47</t>
+  </si>
+  <si>
+    <t>02:d1:11:37:fc:48</t>
+  </si>
+  <si>
+    <t>02:d1:11:37:fc:49</t>
+  </si>
+  <si>
+    <t>02:d1:11:37:fc:50</t>
+  </si>
+  <si>
+    <t>02:d1:11:37:fc:51</t>
+  </si>
+  <si>
+    <t>02:d1:11:37:fc:52</t>
+  </si>
+  <si>
+    <t>02:d1:11:37:fc:53</t>
+  </si>
+  <si>
+    <t>02:d1:11:37:fc:54</t>
+  </si>
+  <si>
+    <t>02:d1:11:37:fc:55</t>
+  </si>
+  <si>
+    <t>02:d1:11:37:fc:56</t>
+  </si>
+  <si>
+    <t>02:d1:11:37:fc:57</t>
+  </si>
+  <si>
+    <t>02:d1:11:37:fc:58</t>
+  </si>
+  <si>
+    <t>02:d1:11:37:fc:59</t>
+  </si>
+  <si>
+    <t>02:d1:11:37:fc:60</t>
+  </si>
+  <si>
+    <t>02:d1:11:37:fc:61</t>
+  </si>
+  <si>
+    <t>02:d1:11:37:fc:62</t>
   </si>
 </sst>
 </file>
@@ -446,7 +521,6 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1019,10 +1093,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Blatt1" enableFormatConditionsCalculation="0"/>
-  <dimension ref="A1:K25"/>
+  <dimension ref="A1:L25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1030,16 +1104,17 @@
     <col min="2" max="2" width="15.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="26.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.83203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.83203125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="8" style="1" customWidth="1"/>
-    <col min="10" max="10" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.83203125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="8" style="1" customWidth="1"/>
+    <col min="11" max="11" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:12">
       <c r="A1" s="2" t="s">
         <v>90</v>
       </c>
@@ -1053,28 +1128,31 @@
         <v>89</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:12">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1089,32 +1167,35 @@
         <v>Freifunk Heppenheim D01</v>
       </c>
       <c r="E2" t="s">
+        <v>133</v>
+      </c>
+      <c r="F2" t="s">
         <v>23</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>24</v>
       </c>
-      <c r="G2" s="1" t="str">
-        <f>LEFT(E2,FIND(".0/",E2))&amp;"1"</f>
+      <c r="H2" s="1" t="str">
+        <f>LEFT(F2,FIND(".0/",F2))&amp;"1"</f>
         <v>10.1.160.1</v>
       </c>
-      <c r="H2" s="1" t="str">
-        <f>LEFT(F2,FIND("::/",F2))&amp;":1"</f>
+      <c r="I2" s="1" t="str">
+        <f>LEFT(G2,FIND("::/",G2))&amp;":1"</f>
         <v>2a03:2260:1010:100::1</v>
       </c>
-      <c r="I2" s="1" t="str">
+      <c r="J2" s="1" t="str">
         <f>"200"&amp;UPPER(RIGHT(A2, 2))</f>
         <v>20001</v>
       </c>
-      <c r="J2" t="s">
-        <v>25</v>
-      </c>
-      <c r="K2" s="1" t="str">
+      <c r="K2" t="s">
+        <v>25</v>
+      </c>
+      <c r="L2" s="1" t="str">
         <f>A2&amp;"/"</f>
         <v>ffhpd01/</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:12">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -1129,32 +1210,35 @@
         <v>Freifunk Moerlenbach D02</v>
       </c>
       <c r="E3" t="s">
+        <v>134</v>
+      </c>
+      <c r="F3" t="s">
         <v>27</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>28</v>
       </c>
-      <c r="G3" s="1" t="str">
-        <f t="shared" ref="G3:G25" si="1">LEFT(E3,FIND(".0/",E3))&amp;"1"</f>
+      <c r="H3" s="1" t="str">
+        <f t="shared" ref="H3:H25" si="1">LEFT(F3,FIND(".0/",F3))&amp;"1"</f>
         <v>10.1.168.1</v>
       </c>
-      <c r="H3" s="1" t="str">
-        <f t="shared" ref="H3:H25" si="2">LEFT(F3,FIND("::/",F3))&amp;":1"</f>
+      <c r="I3" s="1" t="str">
+        <f t="shared" ref="I3:I25" si="2">LEFT(G3,FIND("::/",G3))&amp;":1"</f>
         <v>2a03:2260:1010:200::1</v>
       </c>
-      <c r="I3" s="1" t="str">
-        <f t="shared" ref="I3:I25" si="3">"200"&amp;UPPER(RIGHT(A3, 2))</f>
+      <c r="J3" s="1" t="str">
+        <f t="shared" ref="J3:J25" si="3">"200"&amp;UPPER(RIGHT(A3, 2))</f>
         <v>20002</v>
       </c>
-      <c r="J3" t="s">
-        <v>25</v>
-      </c>
-      <c r="K3" s="1" t="str">
+      <c r="K3" t="s">
+        <v>25</v>
+      </c>
+      <c r="L3" s="1" t="str">
         <f>A3&amp;"/"</f>
         <v>ffhpd02/</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:12">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -1169,32 +1253,35 @@
         <v>Freifunk Einhausen D03</v>
       </c>
       <c r="E4" t="s">
+        <v>135</v>
+      </c>
+      <c r="F4" t="s">
         <v>30</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>31</v>
       </c>
-      <c r="G4" s="1" t="str">
+      <c r="H4" s="1" t="str">
         <f t="shared" si="1"/>
         <v>10.1.176.1</v>
       </c>
-      <c r="H4" s="1" t="str">
+      <c r="I4" s="1" t="str">
         <f t="shared" si="2"/>
         <v>2a03:2260:1010:300::1</v>
       </c>
-      <c r="I4" s="1" t="str">
+      <c r="J4" s="1" t="str">
         <f t="shared" si="3"/>
         <v>20003</v>
       </c>
-      <c r="J4" t="s">
-        <v>25</v>
-      </c>
-      <c r="K4" s="1" t="str">
-        <f t="shared" ref="K4:K25" si="4">A4&amp;"/"</f>
+      <c r="K4" t="s">
+        <v>25</v>
+      </c>
+      <c r="L4" s="1" t="str">
+        <f t="shared" ref="L4:L25" si="4">A4&amp;"/"</f>
         <v>ffhpd03/</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:12">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -1209,32 +1296,35 @@
         <v>Freifunk Bensheim D04</v>
       </c>
       <c r="E5" t="s">
+        <v>136</v>
+      </c>
+      <c r="F5" t="s">
         <v>33</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>34</v>
       </c>
-      <c r="G5" s="1" t="str">
+      <c r="H5" s="1" t="str">
         <f t="shared" si="1"/>
         <v>10.1.184.1</v>
       </c>
-      <c r="H5" s="1" t="str">
+      <c r="I5" s="1" t="str">
         <f t="shared" si="2"/>
         <v>2a03:2260:1010:400::1</v>
       </c>
-      <c r="I5" s="1" t="str">
+      <c r="J5" s="1" t="str">
         <f t="shared" si="3"/>
         <v>20004</v>
       </c>
-      <c r="J5" t="s">
-        <v>25</v>
-      </c>
-      <c r="K5" s="1" t="str">
+      <c r="K5" t="s">
+        <v>25</v>
+      </c>
+      <c r="L5" s="1" t="str">
         <f t="shared" si="4"/>
         <v>ffhpd04/</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:12">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -1249,32 +1339,35 @@
         <v>Freifunk Buerstadt D05</v>
       </c>
       <c r="E6" t="s">
+        <v>137</v>
+      </c>
+      <c r="F6" t="s">
         <v>36</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>37</v>
       </c>
-      <c r="G6" s="1" t="str">
+      <c r="H6" s="1" t="str">
         <f t="shared" si="1"/>
         <v>10.58.0.1</v>
       </c>
-      <c r="H6" s="1" t="str">
+      <c r="I6" s="1" t="str">
         <f t="shared" si="2"/>
         <v>2a03:2260:1010:500::1</v>
       </c>
-      <c r="I6" s="1" t="str">
+      <c r="J6" s="1" t="str">
         <f t="shared" si="3"/>
         <v>20005</v>
       </c>
-      <c r="J6" t="s">
-        <v>25</v>
-      </c>
-      <c r="K6" s="1" t="str">
+      <c r="K6" t="s">
+        <v>25</v>
+      </c>
+      <c r="L6" s="1" t="str">
         <f t="shared" si="4"/>
         <v>ffhpd05/</v>
       </c>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:12">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -1289,32 +1382,35 @@
         <v>Freifunk Hirschhorn D06</v>
       </c>
       <c r="E7" t="s">
+        <v>138</v>
+      </c>
+      <c r="F7" t="s">
         <v>39</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>40</v>
       </c>
-      <c r="G7" s="1" t="str">
+      <c r="H7" s="1" t="str">
         <f t="shared" si="1"/>
         <v>10.58.8.1</v>
       </c>
-      <c r="H7" s="1" t="str">
+      <c r="I7" s="1" t="str">
         <f t="shared" si="2"/>
         <v>2a03:2260:1010:600::1</v>
       </c>
-      <c r="I7" s="1" t="str">
+      <c r="J7" s="1" t="str">
         <f t="shared" si="3"/>
         <v>20006</v>
       </c>
-      <c r="J7" t="s">
-        <v>25</v>
-      </c>
-      <c r="K7" s="1" t="str">
+      <c r="K7" t="s">
+        <v>25</v>
+      </c>
+      <c r="L7" s="1" t="str">
         <f t="shared" si="4"/>
         <v>ffhpd06/</v>
       </c>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:12">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -1329,32 +1425,35 @@
         <v>Freifunk Lampertheim D07</v>
       </c>
       <c r="E8" t="s">
+        <v>139</v>
+      </c>
+      <c r="F8" t="s">
         <v>42</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>43</v>
       </c>
-      <c r="G8" s="1" t="str">
+      <c r="H8" s="1" t="str">
         <f t="shared" si="1"/>
         <v>10.58.16.1</v>
       </c>
-      <c r="H8" s="1" t="str">
+      <c r="I8" s="1" t="str">
         <f t="shared" si="2"/>
         <v>2a03:2260:1010:700::1</v>
       </c>
-      <c r="I8" s="1" t="str">
+      <c r="J8" s="1" t="str">
         <f t="shared" si="3"/>
         <v>20007</v>
       </c>
-      <c r="J8" t="s">
-        <v>25</v>
-      </c>
-      <c r="K8" s="1" t="str">
+      <c r="K8" t="s">
+        <v>25</v>
+      </c>
+      <c r="L8" s="1" t="str">
         <f t="shared" si="4"/>
         <v>ffhpd07/</v>
       </c>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:12">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -1369,32 +1468,35 @@
         <v>Freifunk Lindenfels D08</v>
       </c>
       <c r="E9" t="s">
+        <v>140</v>
+      </c>
+      <c r="F9" t="s">
         <v>45</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
         <v>46</v>
       </c>
-      <c r="G9" s="1" t="str">
+      <c r="H9" s="1" t="str">
         <f t="shared" si="1"/>
         <v>10.58.24.1</v>
       </c>
-      <c r="H9" s="1" t="str">
+      <c r="I9" s="1" t="str">
         <f t="shared" si="2"/>
         <v>2a03:2260:1010:800::1</v>
       </c>
-      <c r="I9" s="1" t="str">
+      <c r="J9" s="1" t="str">
         <f t="shared" si="3"/>
         <v>20008</v>
       </c>
-      <c r="J9" t="s">
-        <v>25</v>
-      </c>
-      <c r="K9" s="1" t="str">
+      <c r="K9" t="s">
+        <v>25</v>
+      </c>
+      <c r="L9" s="1" t="str">
         <f t="shared" si="4"/>
         <v>ffhpd08/</v>
       </c>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:12">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -1409,32 +1511,35 @@
         <v>Freifunk Lorsch D09</v>
       </c>
       <c r="E10" t="s">
+        <v>141</v>
+      </c>
+      <c r="F10" t="s">
         <v>48</v>
       </c>
-      <c r="F10" t="s">
+      <c r="G10" t="s">
         <v>49</v>
       </c>
-      <c r="G10" s="1" t="str">
+      <c r="H10" s="1" t="str">
         <f t="shared" si="1"/>
         <v>10.58.32.1</v>
       </c>
-      <c r="H10" s="1" t="str">
+      <c r="I10" s="1" t="str">
         <f t="shared" si="2"/>
         <v>2a03:2260:1010:900::1</v>
       </c>
-      <c r="I10" s="1" t="str">
+      <c r="J10" s="1" t="str">
         <f t="shared" si="3"/>
         <v>20009</v>
       </c>
-      <c r="J10" t="s">
-        <v>25</v>
-      </c>
-      <c r="K10" s="1" t="str">
+      <c r="K10" t="s">
+        <v>25</v>
+      </c>
+      <c r="L10" s="1" t="str">
         <f t="shared" si="4"/>
         <v>ffhpd09/</v>
       </c>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:12">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -1449,32 +1554,35 @@
         <v>Freifunk Neckarsteinach D10</v>
       </c>
       <c r="E11" t="s">
+        <v>142</v>
+      </c>
+      <c r="F11" t="s">
         <v>51</v>
       </c>
-      <c r="F11" t="s">
+      <c r="G11" t="s">
         <v>52</v>
       </c>
-      <c r="G11" s="1" t="str">
+      <c r="H11" s="1" t="str">
         <f t="shared" si="1"/>
         <v>10.58.40.1</v>
       </c>
-      <c r="H11" s="1" t="str">
+      <c r="I11" s="1" t="str">
         <f t="shared" si="2"/>
         <v>2a03:2260:1010:1000::1</v>
       </c>
-      <c r="I11" s="1" t="str">
+      <c r="J11" s="1" t="str">
         <f t="shared" si="3"/>
         <v>20010</v>
       </c>
-      <c r="J11" t="s">
-        <v>25</v>
-      </c>
-      <c r="K11" s="1" t="str">
+      <c r="K11" t="s">
+        <v>25</v>
+      </c>
+      <c r="L11" s="1" t="str">
         <f t="shared" si="4"/>
         <v>ffhpd10/</v>
       </c>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:12">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -1489,32 +1597,35 @@
         <v>Freifunk Viernheim D11</v>
       </c>
       <c r="E12" t="s">
+        <v>143</v>
+      </c>
+      <c r="F12" t="s">
         <v>54</v>
       </c>
-      <c r="F12" t="s">
+      <c r="G12" t="s">
         <v>55</v>
       </c>
-      <c r="G12" s="1" t="str">
+      <c r="H12" s="1" t="str">
         <f t="shared" si="1"/>
         <v>10.58.48.1</v>
       </c>
-      <c r="H12" s="1" t="str">
+      <c r="I12" s="1" t="str">
         <f t="shared" si="2"/>
         <v>2a03:2260:1010:1100::1</v>
       </c>
-      <c r="I12" s="1" t="str">
+      <c r="J12" s="1" t="str">
         <f t="shared" si="3"/>
         <v>20011</v>
       </c>
-      <c r="J12" t="s">
-        <v>25</v>
-      </c>
-      <c r="K12" s="1" t="str">
+      <c r="K12" t="s">
+        <v>25</v>
+      </c>
+      <c r="L12" s="1" t="str">
         <f t="shared" si="4"/>
         <v>ffhpd11/</v>
       </c>
     </row>
-    <row r="13" spans="1:11">
+    <row r="13" spans="1:12">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -1529,32 +1640,35 @@
         <v>Freifunk Zwingenberg D12</v>
       </c>
       <c r="E13" t="s">
+        <v>144</v>
+      </c>
+      <c r="F13" t="s">
         <v>57</v>
       </c>
-      <c r="F13" t="s">
+      <c r="G13" t="s">
         <v>58</v>
       </c>
-      <c r="G13" s="1" t="str">
+      <c r="H13" s="1" t="str">
         <f t="shared" si="1"/>
         <v>10.58.56.1</v>
       </c>
-      <c r="H13" s="1" t="str">
+      <c r="I13" s="1" t="str">
         <f t="shared" si="2"/>
         <v>2a03:2260:1010:1200::1</v>
       </c>
-      <c r="I13" s="1" t="str">
+      <c r="J13" s="1" t="str">
         <f t="shared" si="3"/>
         <v>20012</v>
       </c>
-      <c r="J13" t="s">
-        <v>25</v>
-      </c>
-      <c r="K13" s="1" t="str">
+      <c r="K13" t="s">
+        <v>25</v>
+      </c>
+      <c r="L13" s="1" t="str">
         <f t="shared" si="4"/>
         <v>ffhpd12/</v>
       </c>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:12">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -1569,32 +1683,35 @@
         <v>Freifunk Abtsteinach D13</v>
       </c>
       <c r="E14" t="s">
+        <v>145</v>
+      </c>
+      <c r="F14" t="s">
         <v>59</v>
       </c>
-      <c r="F14" t="s">
+      <c r="G14" t="s">
         <v>60</v>
       </c>
-      <c r="G14" s="1" t="str">
+      <c r="H14" s="1" t="str">
         <f t="shared" si="1"/>
         <v>10.58.64.1</v>
       </c>
-      <c r="H14" s="1" t="str">
+      <c r="I14" s="1" t="str">
         <f t="shared" si="2"/>
         <v>2a03:2260:1010:1300::1</v>
       </c>
-      <c r="I14" s="1" t="str">
+      <c r="J14" s="1" t="str">
         <f t="shared" si="3"/>
         <v>20013</v>
       </c>
-      <c r="J14" t="s">
-        <v>25</v>
-      </c>
-      <c r="K14" s="1" t="str">
+      <c r="K14" t="s">
+        <v>25</v>
+      </c>
+      <c r="L14" s="1" t="str">
         <f t="shared" si="4"/>
         <v>ffhpd13/</v>
       </c>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:12">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -1609,32 +1726,35 @@
         <v>Freifunk Biblis D14</v>
       </c>
       <c r="E15" t="s">
+        <v>146</v>
+      </c>
+      <c r="F15" t="s">
         <v>62</v>
       </c>
-      <c r="F15" t="s">
+      <c r="G15" t="s">
         <v>63</v>
       </c>
-      <c r="G15" s="1" t="str">
+      <c r="H15" s="1" t="str">
         <f t="shared" si="1"/>
         <v>10.58.72.1</v>
       </c>
-      <c r="H15" s="1" t="str">
+      <c r="I15" s="1" t="str">
         <f t="shared" si="2"/>
         <v>2a03:2260:1010:1400::1</v>
       </c>
-      <c r="I15" s="1" t="str">
+      <c r="J15" s="1" t="str">
         <f t="shared" si="3"/>
         <v>20014</v>
       </c>
-      <c r="J15" t="s">
-        <v>25</v>
-      </c>
-      <c r="K15" s="1" t="str">
+      <c r="K15" t="s">
+        <v>25</v>
+      </c>
+      <c r="L15" s="1" t="str">
         <f t="shared" si="4"/>
         <v>ffhpd14/</v>
       </c>
     </row>
-    <row r="16" spans="1:11">
+    <row r="16" spans="1:12">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -1649,32 +1769,35 @@
         <v>Freifunk Birkenau D15</v>
       </c>
       <c r="E16" t="s">
+        <v>147</v>
+      </c>
+      <c r="F16" t="s">
         <v>65</v>
       </c>
-      <c r="F16" t="s">
+      <c r="G16" t="s">
         <v>66</v>
       </c>
-      <c r="G16" s="1" t="str">
+      <c r="H16" s="1" t="str">
         <f t="shared" si="1"/>
         <v>10.58.80.1</v>
       </c>
-      <c r="H16" s="1" t="str">
+      <c r="I16" s="1" t="str">
         <f t="shared" si="2"/>
         <v>2a03:2260:1010:1500::1</v>
       </c>
-      <c r="I16" s="1" t="str">
+      <c r="J16" s="1" t="str">
         <f t="shared" si="3"/>
         <v>20015</v>
       </c>
-      <c r="J16" t="s">
-        <v>25</v>
-      </c>
-      <c r="K16" s="1" t="str">
+      <c r="K16" t="s">
+        <v>25</v>
+      </c>
+      <c r="L16" s="1" t="str">
         <f t="shared" si="4"/>
         <v>ffhpd15/</v>
       </c>
     </row>
-    <row r="17" spans="1:11">
+    <row r="17" spans="1:12">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -1689,32 +1812,35 @@
         <v>Freifunk Fuerth D16</v>
       </c>
       <c r="E17" t="s">
+        <v>148</v>
+      </c>
+      <c r="F17" t="s">
         <v>68</v>
       </c>
-      <c r="F17" t="s">
+      <c r="G17" t="s">
         <v>69</v>
       </c>
-      <c r="G17" s="1" t="str">
+      <c r="H17" s="1" t="str">
         <f t="shared" si="1"/>
         <v>10.58.88.1</v>
       </c>
-      <c r="H17" s="1" t="str">
+      <c r="I17" s="1" t="str">
         <f t="shared" si="2"/>
         <v>2a03:2260:1010:1600::1</v>
       </c>
-      <c r="I17" s="1" t="str">
+      <c r="J17" s="1" t="str">
         <f t="shared" si="3"/>
         <v>20016</v>
       </c>
-      <c r="J17" t="s">
-        <v>25</v>
-      </c>
-      <c r="K17" s="1" t="str">
+      <c r="K17" t="s">
+        <v>25</v>
+      </c>
+      <c r="L17" s="1" t="str">
         <f t="shared" si="4"/>
         <v>ffhpd16/</v>
       </c>
     </row>
-    <row r="18" spans="1:11">
+    <row r="18" spans="1:12">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -1729,32 +1855,35 @@
         <v>Freifunk Gorxheimertal D17</v>
       </c>
       <c r="E18" t="s">
+        <v>149</v>
+      </c>
+      <c r="F18" t="s">
         <v>71</v>
       </c>
-      <c r="F18" t="s">
+      <c r="G18" t="s">
         <v>72</v>
       </c>
-      <c r="G18" s="1" t="str">
+      <c r="H18" s="1" t="str">
         <f t="shared" si="1"/>
         <v>10.58.96.1</v>
       </c>
-      <c r="H18" s="1" t="str">
+      <c r="I18" s="1" t="str">
         <f t="shared" si="2"/>
         <v>2a03:2260:1010:1700::1</v>
       </c>
-      <c r="I18" s="1" t="str">
+      <c r="J18" s="1" t="str">
         <f t="shared" si="3"/>
         <v>20017</v>
       </c>
-      <c r="J18" t="s">
-        <v>25</v>
-      </c>
-      <c r="K18" s="1" t="str">
+      <c r="K18" t="s">
+        <v>25</v>
+      </c>
+      <c r="L18" s="1" t="str">
         <f t="shared" si="4"/>
         <v>ffhpd17/</v>
       </c>
     </row>
-    <row r="19" spans="1:11">
+    <row r="19" spans="1:12">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -1769,32 +1898,35 @@
         <v>Freifunk Grasellenbach D18</v>
       </c>
       <c r="E19" t="s">
+        <v>150</v>
+      </c>
+      <c r="F19" t="s">
         <v>74</v>
       </c>
-      <c r="F19" t="s">
+      <c r="G19" t="s">
         <v>75</v>
       </c>
-      <c r="G19" s="1" t="str">
+      <c r="H19" s="1" t="str">
         <f t="shared" si="1"/>
         <v>10.58.104.1</v>
       </c>
-      <c r="H19" s="1" t="str">
+      <c r="I19" s="1" t="str">
         <f t="shared" si="2"/>
         <v>2a03:2260:1010:1800::1</v>
       </c>
-      <c r="I19" s="1" t="str">
+      <c r="J19" s="1" t="str">
         <f t="shared" si="3"/>
         <v>20018</v>
       </c>
-      <c r="J19" t="s">
-        <v>25</v>
-      </c>
-      <c r="K19" s="1" t="str">
+      <c r="K19" t="s">
+        <v>25</v>
+      </c>
+      <c r="L19" s="1" t="str">
         <f t="shared" si="4"/>
         <v>ffhpd18/</v>
       </c>
     </row>
-    <row r="20" spans="1:11">
+    <row r="20" spans="1:12">
       <c r="A20" t="s">
         <v>18</v>
       </c>
@@ -1809,32 +1941,35 @@
         <v>Freifunk Gross-Rohrheim D19</v>
       </c>
       <c r="E20" t="s">
+        <v>151</v>
+      </c>
+      <c r="F20" t="s">
         <v>77</v>
       </c>
-      <c r="F20" t="s">
+      <c r="G20" t="s">
         <v>78</v>
       </c>
-      <c r="G20" s="1" t="str">
+      <c r="H20" s="1" t="str">
         <f t="shared" si="1"/>
         <v>10.58.112.1</v>
       </c>
-      <c r="H20" s="1" t="str">
+      <c r="I20" s="1" t="str">
         <f t="shared" si="2"/>
         <v>2a03:2260:1010:1900::1</v>
       </c>
-      <c r="I20" s="1" t="str">
+      <c r="J20" s="1" t="str">
         <f t="shared" si="3"/>
         <v>20019</v>
       </c>
-      <c r="J20" t="s">
-        <v>25</v>
-      </c>
-      <c r="K20" s="1" t="str">
+      <c r="K20" t="s">
+        <v>25</v>
+      </c>
+      <c r="L20" s="1" t="str">
         <f t="shared" si="4"/>
         <v>ffhpd19/</v>
       </c>
     </row>
-    <row r="21" spans="1:11">
+    <row r="21" spans="1:12">
       <c r="A21" t="s">
         <v>19</v>
       </c>
@@ -1849,32 +1984,35 @@
         <v>Freifunk Lautertal D20</v>
       </c>
       <c r="E21" t="s">
+        <v>152</v>
+      </c>
+      <c r="F21" t="s">
         <v>80</v>
       </c>
-      <c r="F21" t="s">
+      <c r="G21" t="s">
         <v>81</v>
       </c>
-      <c r="G21" s="1" t="str">
+      <c r="H21" s="1" t="str">
         <f t="shared" si="1"/>
         <v>10.58.120.1</v>
       </c>
-      <c r="H21" s="1" t="str">
+      <c r="I21" s="1" t="str">
         <f t="shared" si="2"/>
         <v>2a03:2260:1010:2000::1</v>
       </c>
-      <c r="I21" s="1" t="str">
+      <c r="J21" s="1" t="str">
         <f t="shared" si="3"/>
         <v>20020</v>
       </c>
-      <c r="J21" t="s">
-        <v>25</v>
-      </c>
-      <c r="K21" s="1" t="str">
+      <c r="K21" t="s">
+        <v>25</v>
+      </c>
+      <c r="L21" s="1" t="str">
         <f t="shared" si="4"/>
         <v>ffhpd20/</v>
       </c>
     </row>
-    <row r="22" spans="1:11">
+    <row r="22" spans="1:12">
       <c r="A22" t="s">
         <v>20</v>
       </c>
@@ -1889,32 +2027,35 @@
         <v>Freifunk Rimbach D21</v>
       </c>
       <c r="E22" t="s">
+        <v>153</v>
+      </c>
+      <c r="F22" t="s">
         <v>82</v>
       </c>
-      <c r="F22" t="s">
+      <c r="G22" t="s">
         <v>83</v>
       </c>
-      <c r="G22" s="1" t="str">
+      <c r="H22" s="1" t="str">
         <f t="shared" si="1"/>
         <v>10.58.128.1</v>
       </c>
-      <c r="H22" s="1" t="str">
+      <c r="I22" s="1" t="str">
         <f t="shared" si="2"/>
         <v>2a03:2260:1010:2100::1</v>
       </c>
-      <c r="I22" s="1" t="str">
+      <c r="J22" s="1" t="str">
         <f t="shared" si="3"/>
         <v>20021</v>
       </c>
-      <c r="J22" t="s">
-        <v>25</v>
-      </c>
-      <c r="K22" s="1" t="str">
+      <c r="K22" t="s">
+        <v>25</v>
+      </c>
+      <c r="L22" s="1" t="str">
         <f t="shared" si="4"/>
         <v>ffhpd21/</v>
       </c>
     </row>
-    <row r="23" spans="1:11">
+    <row r="23" spans="1:12">
       <c r="A23" t="s">
         <v>21</v>
       </c>
@@ -1929,32 +2070,35 @@
         <v>Freifunk Wald-Michelbach D22</v>
       </c>
       <c r="E23" t="s">
+        <v>154</v>
+      </c>
+      <c r="F23" t="s">
         <v>85</v>
       </c>
-      <c r="F23" t="s">
+      <c r="G23" t="s">
         <v>86</v>
       </c>
-      <c r="G23" s="1" t="str">
+      <c r="H23" s="1" t="str">
         <f t="shared" si="1"/>
         <v>10.58.136.1</v>
       </c>
-      <c r="H23" s="1" t="str">
+      <c r="I23" s="1" t="str">
         <f t="shared" si="2"/>
         <v>2a03:2260:1010:2200::1</v>
       </c>
-      <c r="I23" s="1" t="str">
+      <c r="J23" s="1" t="str">
         <f t="shared" si="3"/>
         <v>20022</v>
       </c>
-      <c r="J23" t="s">
-        <v>25</v>
-      </c>
-      <c r="K23" s="1" t="str">
+      <c r="K23" t="s">
+        <v>25</v>
+      </c>
+      <c r="L23" s="1" t="str">
         <f t="shared" si="4"/>
         <v>ffhpd22/</v>
       </c>
     </row>
-    <row r="24" spans="1:11">
+    <row r="24" spans="1:12">
       <c r="A24" t="s">
         <v>121</v>
       </c>
@@ -1969,32 +2113,35 @@
         <v>Freifunk Exterritorial D23</v>
       </c>
       <c r="E24" t="s">
+        <v>155</v>
+      </c>
+      <c r="F24" t="s">
         <v>122</v>
       </c>
-      <c r="F24" t="s">
+      <c r="G24" t="s">
         <v>123</v>
       </c>
-      <c r="G24" s="1" t="str">
+      <c r="H24" s="1" t="str">
         <f t="shared" si="1"/>
         <v>10.58.144.1</v>
       </c>
-      <c r="H24" s="1" t="str">
+      <c r="I24" s="1" t="str">
         <f t="shared" si="2"/>
         <v>2a03:2260:1010:2300::1</v>
       </c>
-      <c r="I24" s="1" t="str">
+      <c r="J24" s="1" t="str">
         <f t="shared" si="3"/>
         <v>20023</v>
       </c>
-      <c r="J24" t="s">
-        <v>25</v>
-      </c>
-      <c r="K24" s="1" t="str">
+      <c r="K24" t="s">
+        <v>25</v>
+      </c>
+      <c r="L24" s="1" t="str">
         <f t="shared" si="4"/>
         <v>ffhpd23/</v>
       </c>
     </row>
-    <row r="25" spans="1:11">
+    <row r="25" spans="1:12">
       <c r="A25" t="s">
         <v>128</v>
       </c>
@@ -2009,27 +2156,30 @@
         <v>Freifunk Testdomaene D36</v>
       </c>
       <c r="E25" t="s">
+        <v>156</v>
+      </c>
+      <c r="F25" t="s">
         <v>126</v>
       </c>
-      <c r="F25" t="s">
+      <c r="G25" t="s">
         <v>127</v>
       </c>
-      <c r="G25" s="1" t="str">
+      <c r="H25" s="1" t="str">
         <f t="shared" si="1"/>
         <v>10.58.248.1</v>
       </c>
-      <c r="H25" s="1" t="str">
+      <c r="I25" s="1" t="str">
         <f t="shared" si="2"/>
         <v>2a03:2260:1010:3600::1</v>
       </c>
-      <c r="I25" s="1" t="str">
+      <c r="J25" s="1" t="str">
         <f t="shared" si="3"/>
         <v>20036</v>
       </c>
-      <c r="J25" t="s">
-        <v>25</v>
-      </c>
-      <c r="K25" s="1" t="str">
+      <c r="K25" t="s">
+        <v>25</v>
+      </c>
+      <c r="L25" s="1" t="str">
         <f t="shared" si="4"/>
         <v>ffhpd36/</v>
       </c>

</xml_diff>

<commit_message>
new parameter BSSID, trailing slash in parameter ‚firmware‘ removed (not used before)
</commit_message>
<xml_diff>
--- a/domains.xlsx
+++ b/domains.xlsx
@@ -1095,8 +1095,8 @@
   <sheetPr codeName="Blatt1" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:L25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2:L25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1191,8 +1191,8 @@
         <v>25</v>
       </c>
       <c r="L2" s="1" t="str">
-        <f>A2&amp;"/"</f>
-        <v>ffhpd01/</v>
+        <f>A2</f>
+        <v>ffhpd01</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -1234,8 +1234,8 @@
         <v>25</v>
       </c>
       <c r="L3" s="1" t="str">
-        <f>A3&amp;"/"</f>
-        <v>ffhpd02/</v>
+        <f t="shared" ref="L3:L25" si="4">A3</f>
+        <v>ffhpd02</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -1277,8 +1277,8 @@
         <v>25</v>
       </c>
       <c r="L4" s="1" t="str">
-        <f t="shared" ref="L4:L25" si="4">A4&amp;"/"</f>
-        <v>ffhpd03/</v>
+        <f t="shared" si="4"/>
+        <v>ffhpd03</v>
       </c>
     </row>
     <row r="5" spans="1:12">
@@ -1321,7 +1321,7 @@
       </c>
       <c r="L5" s="1" t="str">
         <f t="shared" si="4"/>
-        <v>ffhpd04/</v>
+        <v>ffhpd04</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -1364,7 +1364,7 @@
       </c>
       <c r="L6" s="1" t="str">
         <f t="shared" si="4"/>
-        <v>ffhpd05/</v>
+        <v>ffhpd05</v>
       </c>
     </row>
     <row r="7" spans="1:12">
@@ -1407,7 +1407,7 @@
       </c>
       <c r="L7" s="1" t="str">
         <f t="shared" si="4"/>
-        <v>ffhpd06/</v>
+        <v>ffhpd06</v>
       </c>
     </row>
     <row r="8" spans="1:12">
@@ -1450,7 +1450,7 @@
       </c>
       <c r="L8" s="1" t="str">
         <f t="shared" si="4"/>
-        <v>ffhpd07/</v>
+        <v>ffhpd07</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -1493,7 +1493,7 @@
       </c>
       <c r="L9" s="1" t="str">
         <f t="shared" si="4"/>
-        <v>ffhpd08/</v>
+        <v>ffhpd08</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -1536,7 +1536,7 @@
       </c>
       <c r="L10" s="1" t="str">
         <f t="shared" si="4"/>
-        <v>ffhpd09/</v>
+        <v>ffhpd09</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -1579,7 +1579,7 @@
       </c>
       <c r="L11" s="1" t="str">
         <f t="shared" si="4"/>
-        <v>ffhpd10/</v>
+        <v>ffhpd10</v>
       </c>
     </row>
     <row r="12" spans="1:12">
@@ -1622,7 +1622,7 @@
       </c>
       <c r="L12" s="1" t="str">
         <f t="shared" si="4"/>
-        <v>ffhpd11/</v>
+        <v>ffhpd11</v>
       </c>
     </row>
     <row r="13" spans="1:12">
@@ -1665,7 +1665,7 @@
       </c>
       <c r="L13" s="1" t="str">
         <f t="shared" si="4"/>
-        <v>ffhpd12/</v>
+        <v>ffhpd12</v>
       </c>
     </row>
     <row r="14" spans="1:12">
@@ -1708,7 +1708,7 @@
       </c>
       <c r="L14" s="1" t="str">
         <f t="shared" si="4"/>
-        <v>ffhpd13/</v>
+        <v>ffhpd13</v>
       </c>
     </row>
     <row r="15" spans="1:12">
@@ -1751,7 +1751,7 @@
       </c>
       <c r="L15" s="1" t="str">
         <f t="shared" si="4"/>
-        <v>ffhpd14/</v>
+        <v>ffhpd14</v>
       </c>
     </row>
     <row r="16" spans="1:12">
@@ -1794,7 +1794,7 @@
       </c>
       <c r="L16" s="1" t="str">
         <f t="shared" si="4"/>
-        <v>ffhpd15/</v>
+        <v>ffhpd15</v>
       </c>
     </row>
     <row r="17" spans="1:12">
@@ -1837,7 +1837,7 @@
       </c>
       <c r="L17" s="1" t="str">
         <f t="shared" si="4"/>
-        <v>ffhpd16/</v>
+        <v>ffhpd16</v>
       </c>
     </row>
     <row r="18" spans="1:12">
@@ -1880,7 +1880,7 @@
       </c>
       <c r="L18" s="1" t="str">
         <f t="shared" si="4"/>
-        <v>ffhpd17/</v>
+        <v>ffhpd17</v>
       </c>
     </row>
     <row r="19" spans="1:12">
@@ -1923,7 +1923,7 @@
       </c>
       <c r="L19" s="1" t="str">
         <f t="shared" si="4"/>
-        <v>ffhpd18/</v>
+        <v>ffhpd18</v>
       </c>
     </row>
     <row r="20" spans="1:12">
@@ -1966,7 +1966,7 @@
       </c>
       <c r="L20" s="1" t="str">
         <f t="shared" si="4"/>
-        <v>ffhpd19/</v>
+        <v>ffhpd19</v>
       </c>
     </row>
     <row r="21" spans="1:12">
@@ -2009,7 +2009,7 @@
       </c>
       <c r="L21" s="1" t="str">
         <f t="shared" si="4"/>
-        <v>ffhpd20/</v>
+        <v>ffhpd20</v>
       </c>
     </row>
     <row r="22" spans="1:12">
@@ -2052,7 +2052,7 @@
       </c>
       <c r="L22" s="1" t="str">
         <f t="shared" si="4"/>
-        <v>ffhpd21/</v>
+        <v>ffhpd21</v>
       </c>
     </row>
     <row r="23" spans="1:12">
@@ -2095,7 +2095,7 @@
       </c>
       <c r="L23" s="1" t="str">
         <f t="shared" si="4"/>
-        <v>ffhpd22/</v>
+        <v>ffhpd22</v>
       </c>
     </row>
     <row r="24" spans="1:12">
@@ -2138,7 +2138,7 @@
       </c>
       <c r="L24" s="1" t="str">
         <f t="shared" si="4"/>
-        <v>ffhpd23/</v>
+        <v>ffhpd23</v>
       </c>
     </row>
     <row r="25" spans="1:12">
@@ -2181,7 +2181,7 @@
       </c>
       <c r="L25" s="1" t="str">
         <f t="shared" si="4"/>
-        <v>ffhpd36/</v>
+        <v>ffhpd36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>